<commit_message>
Add methods and refine the text file to load in species info except for the hard stuff from text file
</commit_message>
<xml_diff>
--- a/DynamicCavemanWorld/Assets/Resources/CSV/Species_Stats.xlsx
+++ b/DynamicCavemanWorld/Assets/Resources/CSV/Species_Stats.xlsx
@@ -143,18 +143,6 @@
     <t>50 grassland, 50 savannah</t>
   </si>
   <si>
-    <t>4.94 grazing</t>
-  </si>
-  <si>
-    <t>0.6587 grazing, scrub</t>
-  </si>
-  <si>
-    <t>3.4992 grazing, foiliage, scrub</t>
-  </si>
-  <si>
-    <t>3.2933 grazing</t>
-  </si>
-  <si>
     <t>50 desert, 50 hot_desert</t>
   </si>
   <si>
@@ -176,52 +164,64 @@
     <t>any</t>
   </si>
   <si>
-    <t>0.5763 grazing, foiliage, scrub, seeds</t>
-  </si>
-  <si>
     <t>40 forest, 40 mosoon_forest, 40 swamp, 40 rainforest</t>
   </si>
   <si>
     <t>40 tundra, 40 grassland, 40 boreal, 40 forest, 40 monsoon_forest</t>
   </si>
   <si>
-    <t>0.494 meat</t>
-  </si>
-  <si>
-    <t>0.6175 grazing, scrub, foilage</t>
-  </si>
-  <si>
     <t>60 tundra, 40 grassland, 40 boreal, 40 forest, 40 monsoon_forest, 40 swamp, 60 rainforest, 60 artic_marsh</t>
   </si>
   <si>
     <t>40 savannah, 60 monsoon_forest, 60 rainforest</t>
   </si>
   <si>
-    <t>5.7633 grazing</t>
-  </si>
-  <si>
-    <t>32.9333 grazing, foiliage, scrub</t>
-  </si>
-  <si>
-    <t>54.34 grazing, foiliage, scrub</t>
-  </si>
-  <si>
-    <t>0.4528 grazing</t>
-  </si>
-  <si>
-    <t>2.0995 meat</t>
-  </si>
-  <si>
-    <t>0.2058 meat</t>
-  </si>
-  <si>
-    <t>0.0463 meat</t>
-  </si>
-  <si>
     <t>HabitatPreference</t>
   </si>
   <si>
     <t># (1/8) * %ofagetoreproduce * offspring/year</t>
+  </si>
+  <si>
+    <t>4.94-grazing</t>
+  </si>
+  <si>
+    <t>0.6587-grazing, scrub</t>
+  </si>
+  <si>
+    <t>3.4992-grazing, foiliage, scrub</t>
+  </si>
+  <si>
+    <t>3.2933-grazing</t>
+  </si>
+  <si>
+    <t>0.5763-grazing, foiliage, scrub, seeds</t>
+  </si>
+  <si>
+    <t>0.494-meat</t>
+  </si>
+  <si>
+    <t>0.6175-grazing, scrub, foilage</t>
+  </si>
+  <si>
+    <t>5.7633-grazing</t>
+  </si>
+  <si>
+    <t>32.9333-grazing, foiliage, scrub</t>
+  </si>
+  <si>
+    <t>54.34-grazing, foiliage, scrub</t>
+  </si>
+  <si>
+    <t>0.4528-grazing</t>
+  </si>
+  <si>
+    <t>2.0995-meat</t>
+  </si>
+  <si>
+    <t>0.2058-meat</t>
+  </si>
+  <si>
+    <t>0.0463-meat</t>
   </si>
 </sst>
 </file>
@@ -609,7 +609,7 @@
         <v>12</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>13</v>
@@ -659,7 +659,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>22</v>
@@ -673,7 +673,7 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="D3">
         <v>503.99209999999999</v>
@@ -716,7 +716,7 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="D4">
         <v>79.025959999999998</v>
@@ -734,7 +734,7 @@
         <v>1.55</v>
       </c>
       <c r="I4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
@@ -759,7 +759,7 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D5">
         <v>164.63740000000001</v>
@@ -777,7 +777,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="I5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J5" t="b">
         <v>1</v>
@@ -802,7 +802,7 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="D6">
         <v>235.19630000000001</v>
@@ -845,7 +845,7 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D7">
         <v>56.917499999999997</v>
@@ -863,7 +863,7 @@
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
@@ -888,7 +888,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D8">
         <v>35.212200000000003</v>
@@ -906,7 +906,7 @@
         <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J8" t="b">
         <v>1</v>
@@ -931,7 +931,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D9">
         <v>39.815300000000001</v>
@@ -949,7 +949,7 @@
         <v>2.5</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J9" t="b">
         <v>0</v>
@@ -974,7 +974,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D10">
         <v>235.19630000000001</v>
@@ -992,7 +992,7 @@
         <v>1.75</v>
       </c>
       <c r="I10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J10" t="b">
         <v>0</v>
@@ -1017,7 +1017,7 @@
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D11">
         <v>1679.9737</v>
@@ -1035,7 +1035,7 @@
         <v>1.5</v>
       </c>
       <c r="I11" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="J11" t="b">
         <v>1</v>
@@ -1060,7 +1060,7 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D12">
         <v>2771.9567000000002</v>
@@ -1078,7 +1078,7 @@
         <v>1.5</v>
       </c>
       <c r="I12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J12" t="b">
         <v>1</v>
@@ -1103,7 +1103,7 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D13">
         <v>18.479700000000001</v>
@@ -1121,7 +1121,7 @@
         <v>2.5</v>
       </c>
       <c r="I13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J13" t="b">
         <v>0</v>
@@ -1146,7 +1146,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D14">
         <v>83.998599999999996</v>
@@ -1164,7 +1164,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="I14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J14" t="b">
         <v>0</v>
@@ -1189,7 +1189,7 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D15">
         <v>17.606100000000001</v>
@@ -1207,7 +1207,7 @@
         <v>3.5</v>
       </c>
       <c r="I15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J15" t="b">
         <v>1</v>
@@ -1232,7 +1232,7 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D16">
         <v>2.2233999999999998</v>
@@ -1250,7 +1250,7 @@
         <v>3</v>
       </c>
       <c r="I16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J16" t="b">
         <v>1</v>

</xml_diff>